<commit_message>
Adding Update to Python Datascience work
</commit_message>
<xml_diff>
--- a/Pandas_Data_Analysis/examples/ex1.xlsx
+++ b/Pandas_Data_Analysis/examples/ex1.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Unnamed: 0</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1</t>
+  </si>
   <si>
     <t>a</t>
   </si>
@@ -395,13 +401,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -417,65 +423,89 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
-        <v>5</v>
+      <c r="H2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>7</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
-        <v>6</v>
+      <c r="H3" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
         <v>9</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>11</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
-        <v>7</v>
+      <c r="H4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>